<commit_message>
dates were 2024 but should have been 2025
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2025.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2025.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Ruimte en Milieu\Natuur\Vismigratie\Omgekeerd spuibeheer\2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Github\aangepast-spuibeheer\data\spuibeheer\extern\verwerkt_in_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{297715C9-49E4-4F71-8957-902AF78D1953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{751300C9-22D4-442C-9581-EEFCEBA2AC30}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -156,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -373,13 +372,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -394,7 +389,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -712,32 +706,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769A7D22-BE3E-4510-8E51-02EEB5D40F3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="11" max="11" width="22.6328125" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="6"/>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="34" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -755,7 +749,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
@@ -774,13 +768,13 @@
       <c r="O3" s="9"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="28"/>
       <c r="F4" s="8"/>
       <c r="I4" s="8"/>
       <c r="K4" s="8" t="s">
@@ -789,7 +783,7 @@
       <c r="N4" s="8"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
@@ -803,7 +797,7 @@
       <c r="N5" s="8"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="8"/>
@@ -819,7 +813,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>45352</v>
       </c>
@@ -833,7 +827,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="16">
-        <v>45352</v>
+        <v>45717</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="12" t="s">
@@ -847,12 +841,12 @@
       <c r="O7" s="13"/>
       <c r="P7" s="14"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>45353</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="15"/>
@@ -860,20 +854,20 @@
       <c r="F8" s="17"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="18">
-        <v>45353</v>
+      <c r="I8" s="16">
+        <v>45718</v>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="35" t="s">
         <v>10</v>
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="17"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="19"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P8" s="18"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>45354</v>
       </c>
@@ -886,8 +880,8 @@
       <c r="F9" s="17"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="18">
-        <v>45354</v>
+      <c r="I9" s="16">
+        <v>45719</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>12</v>
@@ -898,9 +892,9 @@
         <v>13</v>
       </c>
       <c r="O9" s="15"/>
-      <c r="P9" s="19"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>45355</v>
       </c>
@@ -913,8 +907,8 @@
       <c r="F10" s="17"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
-      <c r="I10" s="18">
-        <v>45355</v>
+      <c r="I10" s="16">
+        <v>45720</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>14</v>
@@ -925,9 +919,9 @@
         <v>15</v>
       </c>
       <c r="O10" s="15"/>
-      <c r="P10" s="19"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>45356</v>
       </c>
@@ -935,13 +929,13 @@
       <c r="C11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
       <c r="F11" s="17"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="18">
-        <v>45356</v>
+      <c r="I11" s="16">
+        <v>45721</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>14</v>
@@ -952,9 +946,9 @@
         <v>11</v>
       </c>
       <c r="O11" s="15"/>
-      <c r="P11" s="19"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P11" s="18"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>45357</v>
       </c>
@@ -962,13 +956,13 @@
       <c r="C12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="29"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="15"/>
       <c r="F12" s="17"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="18">
-        <v>45357</v>
+      <c r="I12" s="16">
+        <v>45722</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>16</v>
@@ -979,9 +973,9 @@
         <v>15</v>
       </c>
       <c r="O12" s="15"/>
-      <c r="P12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P12" s="18"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>45358</v>
       </c>
@@ -994,8 +988,8 @@
       <c r="F13" s="17"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="18">
-        <v>45358</v>
+      <c r="I13" s="16">
+        <v>45723</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>17</v>
@@ -1006,9 +1000,9 @@
         <v>18</v>
       </c>
       <c r="O13" s="15"/>
-      <c r="P13" s="19"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="18"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>45359</v>
       </c>
@@ -1023,8 +1017,8 @@
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
-      <c r="I14" s="18">
-        <v>45359</v>
+      <c r="I14" s="16">
+        <v>45724</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>17</v>
@@ -1035,14 +1029,14 @@
         <v>19</v>
       </c>
       <c r="O14" s="15"/>
-      <c r="P14" s="19"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P14" s="18"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>45360</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="15"/>
@@ -1050,37 +1044,37 @@
       <c r="F15" s="17"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
-      <c r="I15" s="18">
-        <v>45360</v>
-      </c>
-      <c r="K15" s="26" t="s">
+      <c r="I15" s="16">
+        <v>45725</v>
+      </c>
+      <c r="K15" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
       <c r="N15" s="17"/>
       <c r="O15" s="15"/>
-      <c r="P15" s="19"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P15" s="18"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>45361</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="36" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="15"/>
-      <c r="E16" s="19"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="15" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-      <c r="I16" s="18">
-        <v>45361</v>
-      </c>
-      <c r="K16" s="27" t="s">
+      <c r="I16" s="16">
+        <v>45726</v>
+      </c>
+      <c r="K16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="L16" s="15"/>
@@ -1089,9 +1083,9 @@
         <v>21</v>
       </c>
       <c r="O16" s="15"/>
-      <c r="P16" s="19"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P16" s="18"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>45362</v>
       </c>
@@ -1100,14 +1094,14 @@
         <v>22</v>
       </c>
       <c r="D17" s="15"/>
-      <c r="E17" s="19"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="15" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
-      <c r="I17" s="18">
-        <v>45362</v>
+      <c r="I17" s="16">
+        <v>45727</v>
       </c>
       <c r="K17" s="17" t="s">
         <v>22</v>
@@ -1118,54 +1112,54 @@
         <v>23</v>
       </c>
       <c r="O17" s="15"/>
-      <c r="P17" s="19"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P17" s="18"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
-        <v>45363</v>
+        <v>45728</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="15"/>
-      <c r="E18" s="19"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="18">
-        <v>45363</v>
-      </c>
-      <c r="K18" s="27" t="s">
+      <c r="I18" s="16">
+        <v>45728</v>
+      </c>
+      <c r="K18" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="29"/>
+      <c r="L18" s="27"/>
       <c r="M18" s="15"/>
       <c r="N18" s="17" t="s">
         <v>24</v>
       </c>
       <c r="O18" s="15"/>
-      <c r="P18" s="19"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P18" s="18"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="11">
-        <v>45364</v>
+        <v>45729</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="17" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="15"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="15" t="s">
         <v>25</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
-      <c r="I19" s="18">
-        <v>45364</v>
+      <c r="I19" s="16">
+        <v>45729</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>26</v>
@@ -1176,69 +1170,69 @@
         <v>25</v>
       </c>
       <c r="O19" s="15"/>
-      <c r="P19" s="19"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P19" s="18"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
-        <v>45365</v>
+        <v>45730</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="15"/>
-      <c r="E20" s="19"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="18">
-        <v>45365</v>
-      </c>
-      <c r="K20" s="20" t="s">
+      <c r="I20" s="16">
+        <v>45730</v>
+      </c>
+      <c r="K20" s="19" t="s">
         <v>27</v>
       </c>
       <c r="L20" s="15"/>
-      <c r="M20" s="19"/>
+      <c r="M20" s="18"/>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
-      <c r="P20" s="19"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P20" s="18"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="11">
-        <v>45366</v>
+        <v>45731</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="15"/>
-      <c r="E21" s="19"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="15" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="22">
-        <v>45366</v>
-      </c>
-      <c r="J21" s="23"/>
-      <c r="K21" s="20" t="s">
+      <c r="I21" s="16">
+        <v>45731</v>
+      </c>
+      <c r="J21" s="21"/>
+      <c r="K21" s="19" t="s">
         <v>28</v>
       </c>
       <c r="L21" s="15"/>
-      <c r="M21" s="19"/>
+      <c r="M21" s="18"/>
       <c r="N21" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="15"/>
-      <c r="P21" s="19"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P21" s="18"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
-        <v>45367</v>
+        <v>45732</v>
       </c>
       <c r="B22" s="11"/>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="15"/>
@@ -1246,33 +1240,33 @@
       <c r="F22" s="17"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
-      <c r="I22" s="18">
-        <v>45367</v>
-      </c>
-      <c r="K22" s="26" t="s">
+      <c r="I22" s="16">
+        <v>45732</v>
+      </c>
+      <c r="K22" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
       <c r="N22" s="17"/>
       <c r="O22" s="15"/>
-      <c r="P22" s="19"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P22" s="18"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
-        <v>45368</v>
+        <v>45733</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="15"/>
       <c r="F23" s="17"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="18">
-        <v>45368</v>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="16">
+        <v>45733</v>
       </c>
       <c r="K23" s="17" t="s">
         <v>30</v>
@@ -1281,48 +1275,48 @@
       <c r="M23" s="15"/>
       <c r="N23" s="17"/>
       <c r="O23" s="15"/>
-      <c r="P23" s="19"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P23" s="18"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
-        <v>45369</v>
+        <v>45734</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="15"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="18">
-        <v>45369</v>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="16">
+        <v>45734</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>30</v>
       </c>
       <c r="L24" s="15"/>
-      <c r="M24" s="19"/>
+      <c r="M24" s="18"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
-      <c r="P24" s="19"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P24" s="18"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
-        <v>45370</v>
+        <v>45735</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="29"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="15"/>
       <c r="F25" s="17"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="18">
-        <v>45370</v>
+      <c r="I25" s="16">
+        <v>45735</v>
       </c>
       <c r="J25" s="15"/>
       <c r="K25" s="17" t="s">
@@ -1332,11 +1326,11 @@
       <c r="M25" s="15"/>
       <c r="N25" s="17"/>
       <c r="O25" s="15"/>
-      <c r="P25" s="19"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P25" s="18"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
-        <v>45371</v>
+        <v>45736</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="17" t="s">
@@ -1347,8 +1341,8 @@
       <c r="F26" s="17"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="18">
-        <v>45371</v>
+      <c r="I26" s="16">
+        <v>45736</v>
       </c>
       <c r="J26" s="15"/>
       <c r="K26" s="17" t="s">
@@ -1358,11 +1352,11 @@
       <c r="M26" s="15"/>
       <c r="N26" s="17"/>
       <c r="O26" s="15"/>
-      <c r="P26" s="19"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P26" s="18"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
-        <v>45372</v>
+        <v>45737</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="17" t="s">
@@ -1373,8 +1367,8 @@
       <c r="F27" s="17"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="18">
-        <v>45372</v>
+      <c r="I27" s="16">
+        <v>45737</v>
       </c>
       <c r="J27" s="15"/>
       <c r="K27" s="17" t="s">
@@ -1384,11 +1378,11 @@
       <c r="M27" s="15"/>
       <c r="N27" s="17"/>
       <c r="O27" s="15"/>
-      <c r="P27" s="19"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P27" s="18"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
-        <v>45373</v>
+        <v>45738</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="17" t="s">
@@ -1399,8 +1393,8 @@
       <c r="F28" s="17"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
-      <c r="I28" s="18">
-        <v>45373</v>
+      <c r="I28" s="16">
+        <v>45738</v>
       </c>
       <c r="J28" s="15"/>
       <c r="K28" s="17" t="s">
@@ -1410,14 +1404,14 @@
       <c r="M28" s="15"/>
       <c r="N28" s="17"/>
       <c r="O28" s="15"/>
-      <c r="P28" s="19"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P28" s="18"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
-        <v>45374</v>
+        <v>45739</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="15"/>
@@ -1425,22 +1419,22 @@
       <c r="F29" s="17"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
-      <c r="I29" s="18">
-        <v>45374</v>
+      <c r="I29" s="16">
+        <v>45739</v>
       </c>
       <c r="J29" s="15"/>
-      <c r="K29" s="26" t="s">
+      <c r="K29" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
       <c r="N29" s="17"/>
       <c r="O29" s="15"/>
-      <c r="P29" s="19"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P29" s="18"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
-        <v>45375</v>
+        <v>45740</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="17" t="s">
@@ -1453,8 +1447,8 @@
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
-      <c r="I30" s="18">
-        <v>45375</v>
+      <c r="I30" s="16">
+        <v>45740</v>
       </c>
       <c r="J30" s="15"/>
       <c r="K30" s="17" t="s">
@@ -1466,11 +1460,11 @@
         <v>33</v>
       </c>
       <c r="O30" s="15"/>
-      <c r="P30" s="19"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P30" s="18"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
-        <v>45376</v>
+        <v>45741</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="17" t="s">
@@ -1478,13 +1472,13 @@
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="19" t="s">
         <v>34</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
-      <c r="I31" s="18">
-        <v>45376</v>
+      <c r="I31" s="16">
+        <v>45741</v>
       </c>
       <c r="J31" s="15"/>
       <c r="K31" s="17" t="s">
@@ -1492,15 +1486,15 @@
       </c>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
-      <c r="N31" s="20" t="s">
+      <c r="N31" s="19" t="s">
         <v>34</v>
       </c>
       <c r="O31" s="15"/>
-      <c r="P31" s="19"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P31" s="18"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
-        <v>45377</v>
+        <v>45742</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="17" t="s">
@@ -1508,13 +1502,13 @@
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
-      <c r="I32" s="18">
-        <v>45377</v>
+      <c r="I32" s="16">
+        <v>45742</v>
       </c>
       <c r="J32" s="15"/>
       <c r="K32" s="17" t="s">
@@ -1526,11 +1520,11 @@
         <v>25</v>
       </c>
       <c r="O32" s="15"/>
-      <c r="P32" s="19"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P32" s="18"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="11">
-        <v>45378</v>
+        <v>45743</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="17" t="s">
@@ -1543,8 +1537,8 @@
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="18">
-        <v>45378</v>
+      <c r="I33" s="16">
+        <v>45743</v>
       </c>
       <c r="J33" s="15"/>
       <c r="K33" s="17" t="s">
@@ -1556,14 +1550,14 @@
         <v>35</v>
       </c>
       <c r="O33" s="15"/>
-      <c r="P33" s="19"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P33" s="18"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
-        <v>45379</v>
+        <v>45744</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="15"/>
@@ -1573,8 +1567,8 @@
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
-      <c r="I34" s="18">
-        <v>45379</v>
+      <c r="I34" s="16">
+        <v>45744</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="17" t="s">
@@ -1582,15 +1576,15 @@
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="27" t="s">
+      <c r="N34" s="25" t="s">
         <v>36</v>
       </c>
       <c r="O34" s="15"/>
-      <c r="P34" s="19"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P34" s="18"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="11">
-        <v>45380</v>
+        <v>45745</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="17" t="s">
@@ -1598,11 +1592,11 @@
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="20"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="18">
-        <v>45380</v>
+      <c r="I35" s="16">
+        <v>45745</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="17" t="s">
@@ -1610,39 +1604,39 @@
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
-      <c r="N35" s="20"/>
+      <c r="N35" s="19"/>
       <c r="O35" s="15"/>
-      <c r="P35" s="19"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P35" s="18"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
-        <v>45381</v>
+        <v>45746</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="20"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
-      <c r="I36" s="18">
-        <v>45381</v>
+      <c r="I36" s="16">
+        <v>45746</v>
       </c>
       <c r="J36" s="15"/>
-      <c r="K36" s="26" t="s">
+      <c r="K36" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
-      <c r="N36" s="20"/>
+      <c r="N36" s="19"/>
       <c r="O36" s="15"/>
-      <c r="P36" s="19"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P36" s="18"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="11">
-        <v>45382</v>
+        <v>45747</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="17" t="s">
@@ -1653,8 +1647,8 @@
       <c r="F37" s="17"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
-      <c r="I37" s="18">
-        <v>45382</v>
+      <c r="I37" s="16">
+        <v>45747</v>
       </c>
       <c r="J37" s="15"/>
       <c r="K37" s="17" t="s">
@@ -1664,11 +1658,11 @@
       <c r="M37" s="15"/>
       <c r="N37" s="17"/>
       <c r="O37" s="15"/>
-      <c r="P37" s="19"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P37" s="18"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
-        <v>45383</v>
+        <v>45748</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="17" t="s">
@@ -1679,8 +1673,8 @@
       <c r="F38" s="17"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
-      <c r="I38" s="18">
-        <v>45383</v>
+      <c r="I38" s="16">
+        <v>45748</v>
       </c>
       <c r="J38" s="15"/>
       <c r="K38" s="17" t="s">
@@ -1690,11 +1684,11 @@
       <c r="M38" s="15"/>
       <c r="N38" s="17"/>
       <c r="O38" s="15"/>
-      <c r="P38" s="19"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P38" s="18"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="11">
-        <v>45384</v>
+        <v>45749</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="17" t="s">
@@ -1705,8 +1699,8 @@
       <c r="F39" s="17"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
-      <c r="I39" s="18">
-        <v>45384</v>
+      <c r="I39" s="16">
+        <v>45749</v>
       </c>
       <c r="J39" s="15"/>
       <c r="K39" s="17" t="s">
@@ -1716,11 +1710,11 @@
       <c r="M39" s="15"/>
       <c r="N39" s="17"/>
       <c r="O39" s="15"/>
-      <c r="P39" s="19"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P39" s="18"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
-        <v>45385</v>
+        <v>45750</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="15" t="s">
@@ -1730,8 +1724,8 @@
       <c r="F40" s="17"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
-      <c r="I40" s="18">
-        <v>45385</v>
+      <c r="I40" s="16">
+        <v>45750</v>
       </c>
       <c r="J40" s="15"/>
       <c r="K40" s="17" t="s">
@@ -1741,14 +1735,14 @@
       <c r="M40" s="15"/>
       <c r="N40" s="17"/>
       <c r="O40" s="15"/>
-      <c r="P40" s="19"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P40" s="18"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="11">
-        <v>45386</v>
+        <v>45751</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D41" s="15"/>
@@ -1756,22 +1750,22 @@
       <c r="F41" s="17"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
-      <c r="I41" s="18">
-        <v>45386</v>
+      <c r="I41" s="16">
+        <v>45751</v>
       </c>
       <c r="J41" s="15"/>
-      <c r="K41" s="20" t="s">
+      <c r="K41" s="19" t="s">
         <v>27</v>
       </c>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
       <c r="N41" s="17"/>
       <c r="O41" s="15"/>
-      <c r="P41" s="19"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P41" s="18"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
-        <v>45387</v>
+        <v>45752</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="15" t="s">
@@ -1781,8 +1775,8 @@
       <c r="F42" s="17"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
-      <c r="I42" s="18">
-        <v>45387</v>
+      <c r="I42" s="16">
+        <v>45752</v>
       </c>
       <c r="J42" s="15"/>
       <c r="K42" s="15" t="s">
@@ -1791,37 +1785,37 @@
       <c r="M42" s="15"/>
       <c r="N42" s="17"/>
       <c r="O42" s="15"/>
-      <c r="P42" s="19"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P42" s="18"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="11">
-        <v>45388</v>
+        <v>45753</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="15"/>
-      <c r="E43" s="19"/>
+      <c r="E43" s="18"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
-      <c r="I43" s="18">
-        <v>45388</v>
+      <c r="I43" s="16">
+        <v>45753</v>
       </c>
       <c r="J43" s="15"/>
-      <c r="K43" s="26" t="s">
+      <c r="K43" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43" s="17"/>
       <c r="O43" s="15"/>
-      <c r="P43" s="19"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P43" s="18"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
-        <v>45389</v>
+        <v>45754</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="15" t="s">
@@ -1832,8 +1826,8 @@
       <c r="F44" s="17"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
-      <c r="I44" s="18">
-        <v>45389</v>
+      <c r="I44" s="16">
+        <v>45754</v>
       </c>
       <c r="J44" s="15"/>
       <c r="K44" s="15" t="s">
@@ -1843,11 +1837,11 @@
       <c r="M44" s="15"/>
       <c r="N44" s="17"/>
       <c r="O44" s="15"/>
-      <c r="P44" s="19"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P44" s="18"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="11">
-        <v>45390</v>
+        <v>45755</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="15" t="s">
@@ -1858,8 +1852,8 @@
       <c r="F45" s="17"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
-      <c r="I45" s="18">
-        <v>45390</v>
+      <c r="I45" s="16">
+        <v>45755</v>
       </c>
       <c r="J45" s="15"/>
       <c r="K45" s="15" t="s">
@@ -1869,11 +1863,11 @@
       <c r="M45" s="15"/>
       <c r="N45" s="17"/>
       <c r="O45" s="15"/>
-      <c r="P45" s="19"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P45" s="18"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
-        <v>45391</v>
+        <v>45756</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="15" t="s">
@@ -1884,8 +1878,8 @@
       <c r="F46" s="17"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
-      <c r="I46" s="18">
-        <v>45391</v>
+      <c r="I46" s="16">
+        <v>45756</v>
       </c>
       <c r="J46" s="15"/>
       <c r="K46" s="15" t="s">
@@ -1895,22 +1889,22 @@
       <c r="M46" s="15"/>
       <c r="N46" s="17"/>
       <c r="O46" s="15"/>
-      <c r="P46" s="19"/>
-    </row>
-    <row r="47" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P46" s="18"/>
+    </row>
+    <row r="47" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
-        <v>45392</v>
+        <v>45757</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E47" s="25"/>
+      <c r="E47" s="23"/>
       <c r="F47" s="17"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
-      <c r="I47" s="18">
-        <v>45392</v>
+      <c r="I47" s="16">
+        <v>45757</v>
       </c>
       <c r="J47" s="15"/>
       <c r="K47" s="15" t="s">
@@ -1920,22 +1914,22 @@
       <c r="M47" s="15"/>
       <c r="N47" s="17"/>
       <c r="O47" s="15"/>
-      <c r="P47" s="19"/>
-    </row>
-    <row r="48" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P47" s="18"/>
+    </row>
+    <row r="48" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
-        <v>45393</v>
+        <v>45758</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="25"/>
+      <c r="E48" s="23"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
-      <c r="I48" s="18">
-        <v>45393</v>
+      <c r="I48" s="16">
+        <v>45758</v>
       </c>
       <c r="J48" s="15"/>
       <c r="K48" s="15" t="s">
@@ -1945,38 +1939,38 @@
       <c r="M48" s="15"/>
       <c r="N48" s="17"/>
       <c r="O48" s="15"/>
-      <c r="P48" s="19"/>
-    </row>
-    <row r="49" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P48" s="18"/>
+    </row>
+    <row r="49" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
-        <v>45394</v>
+        <v>45759</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="25"/>
+      <c r="E49" s="23"/>
       <c r="F49" s="17"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
-      <c r="I49" s="18">
-        <v>45394</v>
+      <c r="I49" s="16">
+        <v>45759</v>
       </c>
       <c r="J49" s="15"/>
       <c r="K49" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M49" s="25"/>
+      <c r="M49" s="23"/>
       <c r="N49" s="17"/>
       <c r="O49" s="15"/>
-      <c r="P49" s="19"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P49" s="18"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
-        <v>45395</v>
+        <v>45760</v>
       </c>
       <c r="B50" s="11"/>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="15"/>
@@ -1984,129 +1978,129 @@
       <c r="F50" s="17"/>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
-      <c r="I50" s="18">
-        <v>45395</v>
+      <c r="I50" s="16">
+        <v>45760</v>
       </c>
       <c r="J50" s="15"/>
-      <c r="K50" s="26" t="s">
+      <c r="K50" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
-      <c r="N50" s="20"/>
+      <c r="N50" s="19"/>
       <c r="O50" s="15"/>
-      <c r="P50" s="19"/>
-    </row>
-    <row r="51" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P50" s="18"/>
+    </row>
+    <row r="51" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
-        <v>45396</v>
+        <v>45761</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E51" s="25"/>
+      <c r="E51" s="23"/>
       <c r="F51" s="17"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
-      <c r="I51" s="18">
-        <v>45396</v>
+      <c r="I51" s="16">
+        <v>45761</v>
       </c>
       <c r="J51" s="15"/>
       <c r="K51" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M51" s="25"/>
+      <c r="M51" s="23"/>
       <c r="N51" s="17"/>
       <c r="O51" s="15"/>
-      <c r="P51" s="19"/>
-    </row>
-    <row r="52" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P51" s="18"/>
+    </row>
+    <row r="52" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
-        <v>45397</v>
+        <v>45762</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E52" s="25"/>
+      <c r="E52" s="23"/>
       <c r="F52" s="17"/>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
-      <c r="I52" s="18">
-        <v>45397</v>
+      <c r="I52" s="16">
+        <v>45762</v>
       </c>
       <c r="J52" s="15"/>
       <c r="K52" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M52" s="25"/>
+      <c r="M52" s="23"/>
       <c r="N52" s="17"/>
       <c r="O52" s="15"/>
-      <c r="P52" s="19"/>
-    </row>
-    <row r="53" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P52" s="18"/>
+    </row>
+    <row r="53" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
-        <v>45398</v>
+        <v>45763</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E53" s="25"/>
+      <c r="E53" s="23"/>
       <c r="F53" s="17"/>
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
-      <c r="I53" s="18">
-        <v>45398</v>
+      <c r="I53" s="16">
+        <v>45763</v>
       </c>
       <c r="J53" s="15"/>
       <c r="K53" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M53" s="25"/>
+      <c r="M53" s="23"/>
       <c r="N53" s="17"/>
       <c r="O53" s="15"/>
-      <c r="P53" s="19"/>
-    </row>
-    <row r="54" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P53" s="18"/>
+    </row>
+    <row r="54" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
-        <v>45399</v>
+        <v>45764</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E54" s="25"/>
+      <c r="E54" s="23"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
-      <c r="I54" s="18">
-        <v>45399</v>
+      <c r="I54" s="16">
+        <v>45764</v>
       </c>
       <c r="J54" s="15"/>
       <c r="K54" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M54" s="25"/>
+      <c r="M54" s="23"/>
       <c r="N54" s="17"/>
       <c r="O54" s="15"/>
-      <c r="P54" s="19"/>
-    </row>
-    <row r="55" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P54" s="18"/>
+    </row>
+    <row r="55" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
-        <v>45400</v>
+        <v>45765</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="25"/>
+      <c r="E55" s="23"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
-      <c r="I55" s="18">
-        <v>45400</v>
+      <c r="I55" s="16">
+        <v>45765</v>
       </c>
       <c r="J55" s="15"/>
       <c r="K55" s="15" t="s">
@@ -2116,11 +2110,11 @@
       <c r="M55" s="15"/>
       <c r="N55" s="17"/>
       <c r="O55" s="15"/>
-      <c r="P55" s="19"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P55" s="18"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
-        <v>45401</v>
+        <v>45766</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="15" t="s">
@@ -2131,8 +2125,8 @@
       <c r="F56" s="17"/>
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
-      <c r="I56" s="18">
-        <v>45401</v>
+      <c r="I56" s="16">
+        <v>45766</v>
       </c>
       <c r="J56" s="15"/>
       <c r="K56" s="15" t="s">
@@ -2142,14 +2136,14 @@
       <c r="M56" s="15"/>
       <c r="N56" s="17"/>
       <c r="O56" s="15"/>
-      <c r="P56" s="19"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P56" s="18"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
-        <v>45402</v>
+        <v>45767</v>
       </c>
       <c r="B57" s="11"/>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="15"/>
@@ -2157,22 +2151,22 @@
       <c r="F57" s="17"/>
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
-      <c r="I57" s="18">
-        <v>45402</v>
+      <c r="I57" s="16">
+        <v>45767</v>
       </c>
       <c r="J57" s="15"/>
-      <c r="K57" s="26" t="s">
+      <c r="K57" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
       <c r="N57" s="17"/>
       <c r="O57" s="15"/>
-      <c r="P57" s="19"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P57" s="18"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="11">
-        <v>45403</v>
+        <v>45768</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="15" t="s">
@@ -2183,8 +2177,8 @@
       <c r="F58" s="17"/>
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
-      <c r="I58" s="18">
-        <v>45403</v>
+      <c r="I58" s="16">
+        <v>45768</v>
       </c>
       <c r="J58" s="15"/>
       <c r="K58" s="15" t="s">
@@ -2194,11 +2188,11 @@
       <c r="M58" s="15"/>
       <c r="N58" s="17"/>
       <c r="O58" s="15"/>
-      <c r="P58" s="19"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P58" s="18"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="11">
-        <v>45404</v>
+        <v>45769</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="15" t="s">
@@ -2209,8 +2203,8 @@
       <c r="F59" s="17"/>
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
-      <c r="I59" s="18">
-        <v>45404</v>
+      <c r="I59" s="16">
+        <v>45769</v>
       </c>
       <c r="J59" s="15"/>
       <c r="K59" s="15" t="s">
@@ -2220,11 +2214,11 @@
       <c r="M59" s="15"/>
       <c r="N59" s="17"/>
       <c r="O59" s="15"/>
-      <c r="P59" s="19"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P59" s="18"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="11">
-        <v>45405</v>
+        <v>45770</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="17" t="s">
@@ -2235,8 +2229,8 @@
       <c r="F60" s="17"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
-      <c r="I60" s="18">
-        <v>45405</v>
+      <c r="I60" s="16">
+        <v>45770</v>
       </c>
       <c r="J60" s="15"/>
       <c r="K60" s="17" t="s">
@@ -2246,25 +2240,25 @@
       <c r="M60" s="15"/>
       <c r="N60" s="17"/>
       <c r="O60" s="15"/>
-      <c r="P60" s="19"/>
-    </row>
-    <row r="61" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P60" s="18"/>
+    </row>
+    <row r="61" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="11">
-        <v>45406</v>
-      </c>
-      <c r="B61" s="21"/>
+        <v>45771</v>
+      </c>
+      <c r="B61" s="20"/>
       <c r="C61" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="25"/>
+      <c r="D61" s="23"/>
       <c r="E61" s="15"/>
       <c r="F61" s="17"/>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
-      <c r="I61" s="18">
-        <v>45406</v>
-      </c>
-      <c r="J61" s="19"/>
+      <c r="I61" s="16">
+        <v>45771</v>
+      </c>
+      <c r="J61" s="18"/>
       <c r="K61" s="17" t="s">
         <v>37</v>
       </c>
@@ -2272,11 +2266,11 @@
       <c r="M61" s="15"/>
       <c r="N61" s="17"/>
       <c r="O61" s="15"/>
-      <c r="P61" s="19"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P61" s="18"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
-        <v>45407</v>
+        <v>45772</v>
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="17" t="s">
@@ -2287,8 +2281,8 @@
       <c r="F62" s="17"/>
       <c r="G62" s="15"/>
       <c r="H62" s="15"/>
-      <c r="I62" s="18">
-        <v>45407</v>
+      <c r="I62" s="16">
+        <v>45772</v>
       </c>
       <c r="J62" s="15"/>
       <c r="K62" s="17" t="s">
@@ -2298,11 +2292,11 @@
       <c r="M62" s="15"/>
       <c r="N62" s="17"/>
       <c r="O62" s="15"/>
-      <c r="P62" s="19"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P62" s="18"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="11">
-        <v>45408</v>
+        <v>45773</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="17" t="s">
@@ -2313,8 +2307,8 @@
       <c r="F63" s="17"/>
       <c r="G63" s="15"/>
       <c r="H63" s="15"/>
-      <c r="I63" s="18">
-        <v>45408</v>
+      <c r="I63" s="16">
+        <v>45773</v>
       </c>
       <c r="K63" s="17" t="s">
         <v>37</v>
@@ -2323,14 +2317,14 @@
       <c r="M63" s="15"/>
       <c r="N63" s="17"/>
       <c r="O63" s="15"/>
-      <c r="P63" s="19"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P63" s="18"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="11">
-        <v>45409</v>
+        <v>45774</v>
       </c>
       <c r="B64" s="11"/>
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="15"/>
@@ -2338,21 +2332,21 @@
       <c r="F64" s="17"/>
       <c r="G64" s="15"/>
       <c r="H64" s="15"/>
-      <c r="I64" s="18">
-        <v>45409</v>
-      </c>
-      <c r="K64" s="26" t="s">
+      <c r="I64" s="16">
+        <v>45774</v>
+      </c>
+      <c r="K64" s="24" t="s">
         <v>10</v>
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
-      <c r="N64" s="20"/>
+      <c r="N64" s="19"/>
       <c r="O64" s="15"/>
-      <c r="P64" s="19"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P64" s="18"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="11">
-        <v>45410</v>
+        <v>45775</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="17" t="s">
@@ -2363,33 +2357,33 @@
       <c r="F65" s="17"/>
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
-      <c r="I65" s="18">
-        <v>45410</v>
+      <c r="I65" s="16">
+        <v>45775</v>
       </c>
       <c r="K65" s="17" t="s">
         <v>37</v>
       </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
-      <c r="N65" s="20"/>
+      <c r="N65" s="19"/>
       <c r="O65" s="15"/>
-      <c r="P65" s="19"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P65" s="18"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="11">
-        <v>45411</v>
-      </c>
-      <c r="B66" s="21"/>
+        <v>45776</v>
+      </c>
+      <c r="B66" s="20"/>
       <c r="C66" s="17" t="s">
         <v>37</v>
       </c>
       <c r="D66" s="15"/>
-      <c r="E66" s="19"/>
+      <c r="E66" s="18"/>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
       <c r="H66" s="15"/>
-      <c r="I66" s="18">
-        <v>45411</v>
+      <c r="I66" s="16">
+        <v>45776</v>
       </c>
       <c r="K66" s="17" t="s">
         <v>37</v>
@@ -2398,426 +2392,426 @@
       <c r="M66" s="15"/>
       <c r="N66" s="17"/>
       <c r="O66" s="15"/>
-      <c r="P66" s="19"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P66" s="18"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="11">
-        <v>45412</v>
-      </c>
-      <c r="B67" s="21"/>
+        <v>45777</v>
+      </c>
+      <c r="B67" s="20"/>
       <c r="C67" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D67" s="15"/>
-      <c r="E67" s="19"/>
+      <c r="E67" s="18"/>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="11">
-        <v>45412</v>
+      <c r="H67" s="18"/>
+      <c r="I67" s="16">
+        <v>45777</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L67" s="15"/>
-      <c r="M67" s="19"/>
+      <c r="M67" s="18"/>
       <c r="N67" s="15"/>
       <c r="O67" s="15"/>
-      <c r="P67" s="19"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P67" s="18"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="11">
-        <v>45413</v>
-      </c>
-      <c r="B68" s="21"/>
-      <c r="C68" s="29" t="s">
+        <v>45778</v>
+      </c>
+      <c r="B68" s="20"/>
+      <c r="C68" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D68" s="15"/>
-      <c r="E68" s="19"/>
+      <c r="E68" s="18"/>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="11">
-        <v>45413</v>
+      <c r="H68" s="18"/>
+      <c r="I68" s="16">
+        <v>45778</v>
       </c>
       <c r="J68" s="2"/>
-      <c r="K68" s="29" t="s">
+      <c r="K68" s="27" t="s">
         <v>37</v>
       </c>
       <c r="L68" s="15"/>
-      <c r="M68" s="19"/>
+      <c r="M68" s="18"/>
       <c r="N68" s="15"/>
       <c r="O68" s="15"/>
-      <c r="P68" s="19"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P68" s="18"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="11">
-        <v>45414</v>
+        <v>45779</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D69" s="15"/>
-      <c r="E69" s="19"/>
+      <c r="E69" s="18"/>
       <c r="F69" s="17"/>
       <c r="G69" s="15"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="18">
-        <v>45414</v>
+      <c r="H69" s="18"/>
+      <c r="I69" s="16">
+        <v>45779</v>
       </c>
       <c r="J69" s="2"/>
-      <c r="K69" s="29" t="s">
+      <c r="K69" s="27" t="s">
         <v>37</v>
       </c>
       <c r="L69" s="15"/>
-      <c r="M69" s="19"/>
+      <c r="M69" s="18"/>
       <c r="N69" s="17"/>
       <c r="O69" s="15"/>
-      <c r="P69" s="19"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P69" s="18"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="11">
-        <v>45415</v>
+        <v>45780</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D70" s="15"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="20"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="19"/>
       <c r="G70" s="15"/>
-      <c r="H70" s="19"/>
-      <c r="I70" s="18">
-        <v>45415</v>
+      <c r="H70" s="18"/>
+      <c r="I70" s="16">
+        <v>45780</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L70" s="15"/>
-      <c r="M70" s="19"/>
+      <c r="M70" s="18"/>
       <c r="N70" s="17"/>
       <c r="O70" s="15"/>
-      <c r="P70" s="19"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P70" s="18"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="11">
-        <v>45416</v>
+        <v>45781</v>
       </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="38" t="s">
+      <c r="C71" s="35" t="s">
         <v>10</v>
       </c>
       <c r="D71" s="15"/>
-      <c r="E71" s="19"/>
+      <c r="E71" s="18"/>
       <c r="F71" s="17"/>
       <c r="G71" s="15"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="18">
-        <v>45416</v>
+      <c r="H71" s="18"/>
+      <c r="I71" s="16">
+        <v>45781</v>
       </c>
       <c r="J71" s="2"/>
-      <c r="K71" s="38" t="s">
+      <c r="K71" s="35" t="s">
         <v>10</v>
       </c>
       <c r="L71" s="15"/>
-      <c r="M71" s="19"/>
+      <c r="M71" s="18"/>
       <c r="N71" s="17"/>
       <c r="O71" s="15"/>
-      <c r="P71" s="19"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P71" s="18"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="11">
-        <v>45417</v>
+        <v>45782</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D72" s="15"/>
-      <c r="E72" s="19"/>
+      <c r="E72" s="18"/>
       <c r="F72" s="17"/>
       <c r="G72" s="15"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="18">
-        <v>45417</v>
+      <c r="H72" s="18"/>
+      <c r="I72" s="16">
+        <v>45782</v>
       </c>
       <c r="J72" s="2"/>
       <c r="K72" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L72" s="15"/>
-      <c r="M72" s="19"/>
+      <c r="M72" s="18"/>
       <c r="N72" s="17"/>
       <c r="O72" s="15"/>
-      <c r="P72" s="19"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P72" s="18"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="11">
-        <v>45418</v>
+        <v>45783</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D73" s="15"/>
-      <c r="E73" s="19"/>
+      <c r="E73" s="18"/>
       <c r="F73" s="17"/>
       <c r="G73" s="15"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="18">
-        <v>45418</v>
+      <c r="H73" s="18"/>
+      <c r="I73" s="16">
+        <v>45783</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L73" s="15"/>
-      <c r="M73" s="19"/>
+      <c r="M73" s="18"/>
       <c r="N73" s="17"/>
       <c r="O73" s="15"/>
-      <c r="P73" s="19"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P73" s="18"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="11">
-        <v>45419</v>
+        <v>45784</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D74" s="15"/>
-      <c r="E74" s="19"/>
+      <c r="E74" s="18"/>
       <c r="F74" s="17"/>
       <c r="G74" s="15"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="18">
-        <v>45419</v>
+      <c r="H74" s="18"/>
+      <c r="I74" s="16">
+        <v>45784</v>
       </c>
       <c r="J74" s="2"/>
       <c r="K74" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L74" s="15"/>
-      <c r="M74" s="19"/>
+      <c r="M74" s="18"/>
       <c r="N74" s="17"/>
       <c r="O74" s="15"/>
-      <c r="P74" s="19"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P74" s="18"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="11">
-        <v>45420</v>
+        <v>45785</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D75" s="15"/>
-      <c r="E75" s="19"/>
+      <c r="E75" s="18"/>
       <c r="F75" s="17"/>
       <c r="G75" s="15"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="18">
-        <v>45420</v>
+      <c r="H75" s="18"/>
+      <c r="I75" s="16">
+        <v>45785</v>
       </c>
       <c r="J75" s="2"/>
       <c r="K75" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L75" s="15"/>
-      <c r="M75" s="19"/>
+      <c r="M75" s="18"/>
       <c r="N75" s="17"/>
       <c r="O75" s="15"/>
-      <c r="P75" s="19"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P75" s="18"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="11">
-        <v>45421</v>
+        <v>45786</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D76" s="15"/>
-      <c r="E76" s="19"/>
+      <c r="E76" s="18"/>
       <c r="F76" s="17"/>
       <c r="G76" s="15"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="18">
-        <v>45421</v>
+      <c r="H76" s="18"/>
+      <c r="I76" s="16">
+        <v>45786</v>
       </c>
       <c r="J76" s="2"/>
       <c r="K76" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L76" s="15"/>
-      <c r="M76" s="19"/>
+      <c r="M76" s="18"/>
       <c r="N76" s="17"/>
       <c r="O76" s="15"/>
-      <c r="P76" s="19"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P76" s="18"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="11">
-        <v>45422</v>
+        <v>45787</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D77" s="15"/>
-      <c r="E77" s="19"/>
+      <c r="E77" s="18"/>
       <c r="F77" s="17"/>
       <c r="G77" s="15"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="18">
-        <v>45422</v>
+      <c r="H77" s="18"/>
+      <c r="I77" s="16">
+        <v>45787</v>
       </c>
       <c r="J77" s="2"/>
       <c r="K77" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L77" s="15"/>
-      <c r="M77" s="19"/>
+      <c r="M77" s="18"/>
       <c r="N77" s="17"/>
       <c r="O77" s="15"/>
-      <c r="P77" s="19"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P77" s="18"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="11">
-        <v>45423</v>
+        <v>45788</v>
       </c>
       <c r="B78" s="2"/>
-      <c r="C78" s="38" t="s">
+      <c r="C78" s="35" t="s">
         <v>10</v>
       </c>
       <c r="D78" s="15"/>
-      <c r="E78" s="19"/>
+      <c r="E78" s="18"/>
       <c r="F78" s="17"/>
       <c r="G78" s="15"/>
-      <c r="H78" s="19"/>
-      <c r="I78" s="18">
-        <v>45423</v>
+      <c r="H78" s="18"/>
+      <c r="I78" s="16">
+        <v>45788</v>
       </c>
       <c r="J78" s="2"/>
-      <c r="K78" s="38" t="s">
+      <c r="K78" s="35" t="s">
         <v>10</v>
       </c>
       <c r="L78" s="15"/>
-      <c r="M78" s="19"/>
+      <c r="M78" s="18"/>
       <c r="N78" s="17"/>
       <c r="O78" s="15"/>
-      <c r="P78" s="19"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P78" s="18"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="11">
-        <v>45424</v>
+        <v>45789</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D79" s="15"/>
-      <c r="E79" s="19"/>
+      <c r="E79" s="18"/>
       <c r="F79" s="17"/>
       <c r="G79" s="15"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="18">
-        <v>45424</v>
+      <c r="H79" s="18"/>
+      <c r="I79" s="16">
+        <v>45789</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L79" s="15"/>
-      <c r="M79" s="19"/>
+      <c r="M79" s="18"/>
       <c r="N79" s="17"/>
       <c r="O79" s="15"/>
-      <c r="P79" s="19"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P79" s="18"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="11">
-        <v>45425</v>
+        <v>45790</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D80" s="15"/>
-      <c r="E80" s="19"/>
+      <c r="E80" s="18"/>
       <c r="F80" s="17"/>
       <c r="G80" s="15"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="18">
-        <v>45425</v>
+      <c r="H80" s="18"/>
+      <c r="I80" s="16">
+        <v>45790</v>
       </c>
       <c r="J80" s="2"/>
       <c r="K80" s="17" t="s">
         <v>37</v>
       </c>
       <c r="L80" s="15"/>
-      <c r="M80" s="19"/>
+      <c r="M80" s="18"/>
       <c r="N80" s="17"/>
       <c r="O80" s="15"/>
-      <c r="P80" s="19"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P80" s="18"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="11">
-        <v>45426</v>
+        <v>45791</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D81" s="15"/>
-      <c r="E81" s="19"/>
+      <c r="E81" s="18"/>
       <c r="F81" s="17"/>
       <c r="G81" s="15"/>
-      <c r="H81" s="19"/>
-      <c r="I81" s="18">
-        <v>45426</v>
+      <c r="H81" s="18"/>
+      <c r="I81" s="16">
+        <v>45791</v>
       </c>
       <c r="J81" s="2"/>
       <c r="K81" s="17" t="s">
         <v>37</v>
       </c>
       <c r="L81" s="15"/>
-      <c r="M81" s="19"/>
+      <c r="M81" s="18"/>
       <c r="N81" s="17"/>
       <c r="O81" s="15"/>
-      <c r="P81" s="19"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P81" s="18"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="11">
-        <v>45427</v>
+        <v>45792</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="15" t="s">
         <v>38</v>
       </c>
       <c r="D82" s="15"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="34"/>
-      <c r="H82" s="34"/>
-      <c r="I82" s="35">
-        <v>45427</v>
+      <c r="E82" s="18"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="32"/>
+      <c r="H82" s="32"/>
+      <c r="I82" s="16">
+        <v>45792</v>
       </c>
       <c r="J82" s="5"/>
       <c r="K82" s="15" t="s">
         <v>38</v>
       </c>
       <c r="L82" s="15"/>
-      <c r="M82" s="19"/>
+      <c r="M82" s="18"/>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
       <c r="P82" s="5"/>
     </row>
-    <row r="83" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="28"/>
+    <row r="83" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="26"/>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
@@ -2826,8 +2820,8 @@
       <c r="H83" s="15"/>
       <c r="I83" s="11"/>
       <c r="K83" s="15"/>
-      <c r="L83" s="31"/>
-      <c r="M83" s="32"/>
+      <c r="L83" s="29"/>
+      <c r="M83" s="30"/>
       <c r="N83" s="15"/>
     </row>
   </sheetData>

</xml_diff>